<commit_message>
checked group reports; OK
</commit_message>
<xml_diff>
--- a/doc/individual_report_checking.xlsx
+++ b/doc/individual_report_checking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suhas\Desktop\prjs\cognitive_measures\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBDEA36-FA5D-48F1-94EE-7A31C5997B57}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B8341B-A134-4B74-98BD-E25D19ED651E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2268" windowWidth="23040" windowHeight="7824" xr2:uid="{B45230EC-5FFD-4087-AB00-E8CCC57066AD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="1" xr2:uid="{B45230EC-5FFD-4087-AB00-E8CCC57066AD}"/>
   </bookViews>
   <sheets>
     <sheet name="VA" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="33">
   <si>
     <t>Individual Reports</t>
   </si>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C301E00-8A40-4A02-9EAE-F3F49950E440}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,13 +730,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CB944D-2DCF-42B0-98A0-C54133435BEF}">
   <dimension ref="A1:E1032206"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -908,7 +908,7 @@
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>9</v>
       </c>
@@ -916,7 +916,7 @@
         <v>2.5177</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>10</v>
       </c>
@@ -924,7 +924,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -935,7 +935,7 @@
         <v>2.1032999999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>16</v>
       </c>
@@ -943,7 +943,7 @@
         <v>0.1237</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>32</v>
       </c>
@@ -951,12 +951,17 @@
         <v>-0.17549999999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="1">
         <v>0.89090000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16385" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>